<commit_message>
Se termina version sin darle formato a las hojas
</commit_message>
<xml_diff>
--- a/DocuemntosTitulos/Libro de Control de Folios de Titulos y Grados Electrónicos 2025.xlsx
+++ b/DocuemntosTitulos/Libro de Control de Folios de Titulos y Grados Electrónicos 2025.xlsx
@@ -10,8 +10,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQUETE 211914 HOJA 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQUETE 213229 HOJA 1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQUETE 214627 HOJA 1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQ. T-214627 Hoja 1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQ. T-222042 Hoja 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQ. T-211214 Hoja 1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQ. T-213229 Hoja 1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PAQ. T-211914 Hoja 1" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -326,6 +327,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -340,15 +350,6 @@
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -457,37 +458,23 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -508,17 +495,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,19 +881,19 @@
     <col width="20" customWidth="1" style="46" min="7" max="7"/>
     <col width="15.33203125" customWidth="1" style="47" min="8" max="8"/>
     <col width="19.1640625" customWidth="1" style="47" min="9" max="9"/>
-    <col width="16.5" customWidth="1" style="56" min="10" max="10"/>
+    <col width="16.5" customWidth="1" style="52" min="10" max="10"/>
     <col width="44.33203125" customWidth="1" style="47" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="A1" s="55" t="inlineStr">
+      <c r="A1" s="61" t="inlineStr">
         <is>
           <t>UNIVERSIDAD ETAC ON ALIAT</t>
         </is>
       </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="61" t="inlineStr">
         <is>
           <t>CAMPUS ÚNICO</t>
         </is>
@@ -912,14 +913,14 @@
       <c r="K3" s="1" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="57" t="inlineStr">
+      <c r="A4" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">SERVICIOS ESCOLARES </t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="57" t="inlineStr">
+      <c r="A6" s="51" t="inlineStr">
         <is>
           <t>LIBRO DE CONTROL DE FOLIOS DE TITULOS ELECTRONICOS</t>
         </is>
@@ -932,8 +933,8 @@
       <c r="K7" s="46" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="n"/>
-      <c r="C8" s="45" t="n"/>
+      <c r="A8" s="48" t="n"/>
+      <c r="C8" s="48" t="n"/>
       <c r="I8" s="4" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -945,8 +946,8 @@
       <c r="K8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="45" t="n"/>
-      <c r="C9" s="45" t="n"/>
+      <c r="A9" s="48" t="n"/>
+      <c r="C9" s="48" t="n"/>
       <c r="I9" s="4" t="inlineStr">
         <is>
           <t>HOJA</t>
@@ -960,18 +961,18 @@
       <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="45" t="n"/>
-      <c r="C10" s="45" t="n"/>
-      <c r="I10" s="45" t="n"/>
+      <c r="A10" s="48" t="n"/>
+      <c r="C10" s="48" t="n"/>
+      <c r="I10" s="48" t="n"/>
       <c r="J10" s="39" t="n"/>
-      <c r="K10" s="45" t="n"/>
+      <c r="K10" s="48" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="n"/>
-      <c r="C11" s="45" t="n"/>
-      <c r="I11" s="45" t="n"/>
+      <c r="A11" s="48" t="n"/>
+      <c r="C11" s="48" t="n"/>
+      <c r="I11" s="48" t="n"/>
       <c r="J11" s="39" t="n"/>
-      <c r="K11" s="45" t="n"/>
+      <c r="K11" s="48" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="n"/>
@@ -987,74 +988,74 @@
       <c r="K12" s="9" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="61" t="inlineStr">
+      <c r="A13" s="55" t="inlineStr">
         <is>
           <t>NUM. PROG.</t>
         </is>
       </c>
-      <c r="B13" s="58" t="inlineStr">
+      <c r="B13" s="49" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C13" s="58" t="inlineStr">
+      <c r="C13" s="49" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D13" s="58" t="inlineStr">
+      <c r="D13" s="49" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E13" s="51" t="inlineStr">
+      <c r="E13" s="63" t="inlineStr">
         <is>
           <t>CLAVE DE CARRERA</t>
         </is>
       </c>
-      <c r="F13" s="59" t="inlineStr">
+      <c r="F13" s="53" t="inlineStr">
         <is>
           <t>FOLIO DE CONTROL</t>
         </is>
       </c>
-      <c r="G13" s="53" t="inlineStr">
+      <c r="G13" s="65" t="inlineStr">
         <is>
           <t>LUGAR DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="H13" s="61" t="inlineStr">
+      <c r="H13" s="55" t="inlineStr">
         <is>
           <t>FECHA DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="I13" s="64" t="inlineStr">
+      <c r="I13" s="58" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J13" s="48" t="inlineStr">
+      <c r="J13" s="62" t="inlineStr">
         <is>
           <t>CLAVE DE INSTITUCIÓN</t>
         </is>
       </c>
-      <c r="K13" s="61" t="inlineStr">
+      <c r="K13" s="55" t="inlineStr">
         <is>
           <t>FOLIO DIGITAL</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="n"/>
-      <c r="B14" s="49" t="n"/>
-      <c r="C14" s="49" t="n"/>
-      <c r="D14" s="49" t="n"/>
-      <c r="E14" s="52" t="n"/>
-      <c r="F14" s="60" t="n"/>
-      <c r="G14" s="54" t="n"/>
-      <c r="H14" s="49" t="n"/>
-      <c r="I14" s="65" t="n"/>
-      <c r="J14" s="49" t="n"/>
-      <c r="K14" s="49" t="n"/>
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="50" t="n"/>
+      <c r="C14" s="50" t="n"/>
+      <c r="D14" s="50" t="n"/>
+      <c r="E14" s="64" t="n"/>
+      <c r="F14" s="54" t="n"/>
+      <c r="G14" s="66" t="n"/>
+      <c r="H14" s="50" t="n"/>
+      <c r="I14" s="59" t="n"/>
+      <c r="J14" s="50" t="n"/>
+      <c r="K14" s="50" t="n"/>
     </row>
     <row r="15" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A15" s="22" t="n">
@@ -1226,19 +1227,19 @@
       <c r="K23" s="15" t="n"/>
     </row>
     <row r="24" ht="20.25" customFormat="1" customHeight="1" s="47">
-      <c r="A24" s="52" t="n">
+      <c r="A24" s="64" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="60" t="n"/>
-      <c r="C24" s="60" t="n"/>
-      <c r="D24" s="60" t="n"/>
+      <c r="B24" s="54" t="n"/>
+      <c r="C24" s="54" t="n"/>
+      <c r="D24" s="54" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="17" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="28" t="n"/>
-      <c r="I24" s="60" t="n"/>
+      <c r="I24" s="54" t="n"/>
       <c r="J24" s="38" t="n"/>
-      <c r="K24" s="60" t="n"/>
+      <c r="K24" s="54" t="n"/>
     </row>
     <row r="25" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A25" s="31" t="n">
@@ -1259,31 +1260,31 @@
       <c r="A26" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="60" t="n"/>
-      <c r="C26" s="60" t="n"/>
-      <c r="D26" s="60" t="n"/>
+      <c r="B26" s="54" t="n"/>
+      <c r="C26" s="54" t="n"/>
+      <c r="D26" s="54" t="n"/>
       <c r="E26" s="24" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="27" t="n"/>
       <c r="H26" s="28" t="n"/>
-      <c r="I26" s="60" t="n"/>
+      <c r="I26" s="54" t="n"/>
       <c r="J26" s="38" t="n"/>
-      <c r="K26" s="60" t="n"/>
+      <c r="K26" s="54" t="n"/>
     </row>
     <row r="27" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A27" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="49" t="n"/>
-      <c r="C27" s="49" t="n"/>
-      <c r="D27" s="49" t="n"/>
-      <c r="E27" s="52" t="n"/>
+      <c r="B27" s="50" t="n"/>
+      <c r="C27" s="50" t="n"/>
+      <c r="D27" s="50" t="n"/>
+      <c r="E27" s="64" t="n"/>
       <c r="F27" s="17" t="n"/>
-      <c r="G27" s="54" t="n"/>
+      <c r="G27" s="66" t="n"/>
       <c r="H27" s="20" t="n"/>
-      <c r="I27" s="49" t="n"/>
+      <c r="I27" s="50" t="n"/>
       <c r="J27" s="38" t="n"/>
-      <c r="K27" s="49" t="n"/>
+      <c r="K27" s="50" t="n"/>
     </row>
     <row r="28" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A28" s="11" t="n">
@@ -1398,7 +1399,7 @@
       <c r="C35" s="11" t="n"/>
       <c r="D35" s="11" t="n"/>
       <c r="E35" s="11" t="n"/>
-      <c r="F35" s="49" t="n"/>
+      <c r="F35" s="50" t="n"/>
       <c r="G35" s="11" t="n"/>
       <c r="H35" s="5" t="n"/>
       <c r="I35" s="11" t="n"/>
@@ -1490,12 +1491,12 @@
       <c r="G41" s="12" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="66" t="n"/>
-      <c r="C42" s="66" t="n"/>
-      <c r="D42" s="66" t="n"/>
-      <c r="E42" s="66" t="n"/>
-      <c r="F42" s="66" t="n"/>
-      <c r="G42" s="50" t="n"/>
+      <c r="A42" s="60" t="n"/>
+      <c r="C42" s="60" t="n"/>
+      <c r="D42" s="60" t="n"/>
+      <c r="E42" s="60" t="n"/>
+      <c r="F42" s="60" t="n"/>
+      <c r="G42" s="45" t="n"/>
       <c r="I42" s="46" t="n"/>
       <c r="J42" s="40" t="n"/>
       <c r="K42" s="9" t="n"/>
@@ -1519,12 +1520,12 @@
       <c r="I50" s="43" t="n"/>
     </row>
     <row r="51">
-      <c r="C51" s="62" t="inlineStr">
+      <c r="C51" s="56" t="inlineStr">
         <is>
           <t>Mtra. Lilibeth Hernández Alba</t>
         </is>
       </c>
-      <c r="D51" s="63" t="n"/>
+      <c r="D51" s="57" t="n"/>
       <c r="G51" s="47" t="inlineStr">
         <is>
           <t>Mtra. Dely Karolina Urbano Sanchez</t>
@@ -1532,12 +1533,12 @@
       </c>
     </row>
     <row r="52">
-      <c r="C52" s="50" t="inlineStr">
+      <c r="C52" s="45" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SEVICIOS ESCOLARES</t>
         </is>
       </c>
-      <c r="G52" s="50" t="inlineStr">
+      <c r="G52" s="45" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -1547,11 +1548,11 @@
   <mergeCells count="29">
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="J13:J14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C11:H11"/>
@@ -1603,19 +1604,19 @@
     <col width="20" customWidth="1" style="46" min="7" max="7"/>
     <col width="15.33203125" customWidth="1" style="47" min="8" max="8"/>
     <col width="19.1640625" customWidth="1" style="47" min="9" max="9"/>
-    <col width="16.5" customWidth="1" style="56" min="10" max="10"/>
+    <col width="16.5" customWidth="1" style="52" min="10" max="10"/>
     <col width="44.33203125" customWidth="1" style="47" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="A1" s="55" t="inlineStr">
+      <c r="A1" s="61" t="inlineStr">
         <is>
           <t>UNIVERSIDAD ETAC ON ALIAT</t>
         </is>
       </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="61" t="inlineStr">
         <is>
           <t>CAMPUS ÚNICO</t>
         </is>
@@ -1635,14 +1636,14 @@
       <c r="K3" s="1" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="57" t="inlineStr">
+      <c r="A4" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">SERVICIOS ESCOLARES </t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="57" t="inlineStr">
+      <c r="A6" s="51" t="inlineStr">
         <is>
           <t>LIBRO DE CONTROL DE FOLIOS DE TITULOS ELECTRONICOS</t>
         </is>
@@ -1655,8 +1656,8 @@
       <c r="K7" s="46" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="n"/>
-      <c r="C8" s="45" t="n"/>
+      <c r="A8" s="48" t="n"/>
+      <c r="C8" s="48" t="n"/>
       <c r="I8" s="4" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -1668,8 +1669,8 @@
       <c r="K8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="45" t="n"/>
-      <c r="C9" s="45" t="n"/>
+      <c r="A9" s="48" t="n"/>
+      <c r="C9" s="48" t="n"/>
       <c r="I9" s="4" t="inlineStr">
         <is>
           <t>HOJA</t>
@@ -1683,18 +1684,18 @@
       <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="45" t="n"/>
-      <c r="C10" s="45" t="n"/>
-      <c r="I10" s="45" t="n"/>
+      <c r="A10" s="48" t="n"/>
+      <c r="C10" s="48" t="n"/>
+      <c r="I10" s="48" t="n"/>
       <c r="J10" s="39" t="n"/>
-      <c r="K10" s="45" t="n"/>
+      <c r="K10" s="48" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="n"/>
-      <c r="C11" s="45" t="n"/>
-      <c r="I11" s="45" t="n"/>
+      <c r="A11" s="48" t="n"/>
+      <c r="C11" s="48" t="n"/>
+      <c r="I11" s="48" t="n"/>
       <c r="J11" s="39" t="n"/>
-      <c r="K11" s="45" t="n"/>
+      <c r="K11" s="48" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="n"/>
@@ -1710,74 +1711,74 @@
       <c r="K12" s="9" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="61" t="inlineStr">
+      <c r="A13" s="55" t="inlineStr">
         <is>
           <t>NUM. PROG.</t>
         </is>
       </c>
-      <c r="B13" s="58" t="inlineStr">
+      <c r="B13" s="49" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C13" s="58" t="inlineStr">
+      <c r="C13" s="49" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D13" s="58" t="inlineStr">
+      <c r="D13" s="49" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E13" s="51" t="inlineStr">
+      <c r="E13" s="63" t="inlineStr">
         <is>
           <t>CLAVE DE CARRERA</t>
         </is>
       </c>
-      <c r="F13" s="59" t="inlineStr">
+      <c r="F13" s="53" t="inlineStr">
         <is>
           <t>FOLIO DE CONTROL</t>
         </is>
       </c>
-      <c r="G13" s="53" t="inlineStr">
+      <c r="G13" s="65" t="inlineStr">
         <is>
           <t>LUGAR DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="H13" s="61" t="inlineStr">
+      <c r="H13" s="55" t="inlineStr">
         <is>
           <t>FECHA DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="I13" s="64" t="inlineStr">
+      <c r="I13" s="58" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J13" s="48" t="inlineStr">
+      <c r="J13" s="62" t="inlineStr">
         <is>
           <t>CLAVE DE INSTITUCIÓN</t>
         </is>
       </c>
-      <c r="K13" s="61" t="inlineStr">
+      <c r="K13" s="55" t="inlineStr">
         <is>
           <t>FOLIO DIGITAL</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="n"/>
-      <c r="B14" s="49" t="n"/>
-      <c r="C14" s="49" t="n"/>
-      <c r="D14" s="49" t="n"/>
-      <c r="E14" s="52" t="n"/>
-      <c r="F14" s="60" t="n"/>
-      <c r="G14" s="54" t="n"/>
-      <c r="H14" s="49" t="n"/>
-      <c r="I14" s="65" t="n"/>
-      <c r="J14" s="49" t="n"/>
-      <c r="K14" s="49" t="n"/>
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="50" t="n"/>
+      <c r="C14" s="50" t="n"/>
+      <c r="D14" s="50" t="n"/>
+      <c r="E14" s="64" t="n"/>
+      <c r="F14" s="54" t="n"/>
+      <c r="G14" s="66" t="n"/>
+      <c r="H14" s="50" t="n"/>
+      <c r="I14" s="59" t="n"/>
+      <c r="J14" s="50" t="n"/>
+      <c r="K14" s="50" t="n"/>
     </row>
     <row r="15" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A15" s="22" t="n">
@@ -1983,19 +1984,19 @@
       <c r="K23" s="15" t="n"/>
     </row>
     <row r="24" ht="20.25" customFormat="1" customHeight="1" s="47">
-      <c r="A24" s="52" t="n">
+      <c r="A24" s="64" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="60" t="n"/>
-      <c r="C24" s="60" t="n"/>
-      <c r="D24" s="60" t="n"/>
+      <c r="B24" s="54" t="n"/>
+      <c r="C24" s="54" t="n"/>
+      <c r="D24" s="54" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="17" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="28" t="n"/>
-      <c r="I24" s="60" t="n"/>
+      <c r="I24" s="54" t="n"/>
       <c r="J24" s="38" t="n"/>
-      <c r="K24" s="60" t="n"/>
+      <c r="K24" s="54" t="n"/>
     </row>
     <row r="25" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A25" s="31" t="n">
@@ -2016,31 +2017,31 @@
       <c r="A26" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="60" t="n"/>
-      <c r="C26" s="60" t="n"/>
-      <c r="D26" s="60" t="n"/>
+      <c r="B26" s="54" t="n"/>
+      <c r="C26" s="54" t="n"/>
+      <c r="D26" s="54" t="n"/>
       <c r="E26" s="24" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="27" t="n"/>
       <c r="H26" s="28" t="n"/>
-      <c r="I26" s="60" t="n"/>
+      <c r="I26" s="54" t="n"/>
       <c r="J26" s="38" t="n"/>
-      <c r="K26" s="60" t="n"/>
+      <c r="K26" s="54" t="n"/>
     </row>
     <row r="27" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A27" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="49" t="n"/>
-      <c r="C27" s="49" t="n"/>
-      <c r="D27" s="49" t="n"/>
-      <c r="E27" s="52" t="n"/>
+      <c r="B27" s="50" t="n"/>
+      <c r="C27" s="50" t="n"/>
+      <c r="D27" s="50" t="n"/>
+      <c r="E27" s="64" t="n"/>
       <c r="F27" s="17" t="n"/>
-      <c r="G27" s="54" t="n"/>
+      <c r="G27" s="66" t="n"/>
       <c r="H27" s="20" t="n"/>
-      <c r="I27" s="49" t="n"/>
+      <c r="I27" s="50" t="n"/>
       <c r="J27" s="38" t="n"/>
-      <c r="K27" s="49" t="n"/>
+      <c r="K27" s="50" t="n"/>
     </row>
     <row r="28" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A28" s="11" t="n">
@@ -2155,7 +2156,7 @@
       <c r="C35" s="11" t="n"/>
       <c r="D35" s="11" t="n"/>
       <c r="E35" s="11" t="n"/>
-      <c r="F35" s="49" t="n"/>
+      <c r="F35" s="50" t="n"/>
       <c r="G35" s="11" t="n"/>
       <c r="H35" s="5" t="n"/>
       <c r="I35" s="11" t="n"/>
@@ -2247,12 +2248,12 @@
       <c r="G41" s="12" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="66" t="n"/>
-      <c r="C42" s="66" t="n"/>
-      <c r="D42" s="66" t="n"/>
-      <c r="E42" s="66" t="n"/>
-      <c r="F42" s="66" t="n"/>
-      <c r="G42" s="50" t="n"/>
+      <c r="A42" s="60" t="n"/>
+      <c r="C42" s="60" t="n"/>
+      <c r="D42" s="60" t="n"/>
+      <c r="E42" s="60" t="n"/>
+      <c r="F42" s="60" t="n"/>
+      <c r="G42" s="45" t="n"/>
       <c r="I42" s="46" t="n"/>
       <c r="J42" s="40" t="n"/>
       <c r="K42" s="9" t="n"/>
@@ -2274,18 +2275,18 @@
       <c r="G50" s="47" t="n"/>
     </row>
     <row r="51">
-      <c r="C51" s="62" t="inlineStr">
+      <c r="C51" s="56" t="inlineStr">
         <is>
           <t>Mtra. Lilibeth Hernández Alba</t>
         </is>
       </c>
-      <c r="D51" s="63" t="n"/>
+      <c r="D51" s="57" t="n"/>
       <c r="G51" s="44" t="n"/>
       <c r="H51" s="43" t="n"/>
       <c r="I51" s="43" t="n"/>
     </row>
     <row r="52">
-      <c r="C52" s="50" t="inlineStr">
+      <c r="C52" s="45" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SEVICIOS ESCOLARES</t>
         </is>
@@ -2297,7 +2298,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="G53" s="50" t="inlineStr">
+      <c r="G53" s="45" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -2308,11 +2309,11 @@
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G42:H42"/>
     <mergeCell ref="G53:I53"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G42:H42"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C11:H11"/>
@@ -2364,19 +2365,19 @@
     <col width="20" customWidth="1" style="46" min="7" max="7"/>
     <col width="15.33203125" customWidth="1" style="47" min="8" max="8"/>
     <col width="19.1640625" customWidth="1" style="47" min="9" max="9"/>
-    <col width="16.5" customWidth="1" style="56" min="10" max="10"/>
+    <col width="16.5" customWidth="1" style="52" min="10" max="10"/>
     <col width="44.33203125" customWidth="1" style="47" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="A1" s="55" t="inlineStr">
+      <c r="A1" s="61" t="inlineStr">
         <is>
           <t>UNIVERSIDAD ETAC ON ALIAT</t>
         </is>
       </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="61" t="inlineStr">
         <is>
           <t>CAMPUS ÚNICO</t>
         </is>
@@ -2396,14 +2397,14 @@
       <c r="K3" s="1" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="57" t="inlineStr">
+      <c r="A4" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">SERVICIOS ESCOLARES </t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="57" t="inlineStr">
+      <c r="A6" s="51" t="inlineStr">
         <is>
           <t>LIBRO DE CONTROL DE FOLIOS DE TITULOS ELECTRONICOS</t>
         </is>
@@ -2416,8 +2417,8 @@
       <c r="K7" s="46" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="n"/>
-      <c r="C8" s="45" t="n"/>
+      <c r="A8" s="48" t="n"/>
+      <c r="C8" s="48" t="n"/>
       <c r="I8" s="4" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -2429,8 +2430,8 @@
       <c r="K8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="45" t="n"/>
-      <c r="C9" s="45" t="n"/>
+      <c r="A9" s="48" t="n"/>
+      <c r="C9" s="48" t="n"/>
       <c r="I9" s="4" t="inlineStr">
         <is>
           <t>HOJA</t>
@@ -2444,18 +2445,18 @@
       <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="45" t="n"/>
-      <c r="C10" s="45" t="n"/>
-      <c r="I10" s="45" t="n"/>
+      <c r="A10" s="48" t="n"/>
+      <c r="C10" s="48" t="n"/>
+      <c r="I10" s="48" t="n"/>
       <c r="J10" s="39" t="n"/>
-      <c r="K10" s="45" t="n"/>
+      <c r="K10" s="48" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="n"/>
-      <c r="C11" s="45" t="n"/>
-      <c r="I11" s="45" t="n"/>
+      <c r="A11" s="48" t="n"/>
+      <c r="C11" s="48" t="n"/>
+      <c r="I11" s="48" t="n"/>
       <c r="J11" s="39" t="n"/>
-      <c r="K11" s="45" t="n"/>
+      <c r="K11" s="48" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="n"/>
@@ -2471,74 +2472,74 @@
       <c r="K12" s="9" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="61" t="inlineStr">
+      <c r="A13" s="55" t="inlineStr">
         <is>
           <t>NUM. PROG.</t>
         </is>
       </c>
-      <c r="B13" s="58" t="inlineStr">
+      <c r="B13" s="49" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C13" s="58" t="inlineStr">
+      <c r="C13" s="49" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D13" s="58" t="inlineStr">
+      <c r="D13" s="49" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E13" s="51" t="inlineStr">
+      <c r="E13" s="63" t="inlineStr">
         <is>
           <t>CLAVE DE CARRERA</t>
         </is>
       </c>
-      <c r="F13" s="59" t="inlineStr">
+      <c r="F13" s="53" t="inlineStr">
         <is>
           <t>FOLIO DE CONTROL</t>
         </is>
       </c>
-      <c r="G13" s="53" t="inlineStr">
+      <c r="G13" s="65" t="inlineStr">
         <is>
           <t>LUGAR DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="H13" s="61" t="inlineStr">
+      <c r="H13" s="55" t="inlineStr">
         <is>
           <t>FECHA DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="I13" s="64" t="inlineStr">
+      <c r="I13" s="58" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J13" s="48" t="inlineStr">
+      <c r="J13" s="62" t="inlineStr">
         <is>
           <t>CLAVE DE INSTITUCIÓN</t>
         </is>
       </c>
-      <c r="K13" s="61" t="inlineStr">
+      <c r="K13" s="55" t="inlineStr">
         <is>
           <t>FOLIO DIGITAL</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="n"/>
-      <c r="B14" s="49" t="n"/>
-      <c r="C14" s="49" t="n"/>
-      <c r="D14" s="49" t="n"/>
-      <c r="E14" s="52" t="n"/>
-      <c r="F14" s="60" t="n"/>
-      <c r="G14" s="54" t="n"/>
-      <c r="H14" s="49" t="n"/>
-      <c r="I14" s="65" t="n"/>
-      <c r="J14" s="49" t="n"/>
-      <c r="K14" s="49" t="n"/>
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="50" t="n"/>
+      <c r="C14" s="50" t="n"/>
+      <c r="D14" s="50" t="n"/>
+      <c r="E14" s="64" t="n"/>
+      <c r="F14" s="54" t="n"/>
+      <c r="G14" s="66" t="n"/>
+      <c r="H14" s="50" t="n"/>
+      <c r="I14" s="59" t="n"/>
+      <c r="J14" s="50" t="n"/>
+      <c r="K14" s="50" t="n"/>
     </row>
     <row r="15" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A15" s="22" t="n">
@@ -2744,19 +2745,19 @@
       <c r="K23" s="15" t="n"/>
     </row>
     <row r="24" ht="20.25" customFormat="1" customHeight="1" s="47">
-      <c r="A24" s="52" t="n">
+      <c r="A24" s="64" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="60" t="n"/>
-      <c r="C24" s="60" t="n"/>
-      <c r="D24" s="60" t="n"/>
+      <c r="B24" s="54" t="n"/>
+      <c r="C24" s="54" t="n"/>
+      <c r="D24" s="54" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="17" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="28" t="n"/>
-      <c r="I24" s="60" t="n"/>
+      <c r="I24" s="54" t="n"/>
       <c r="J24" s="38" t="n"/>
-      <c r="K24" s="60" t="n"/>
+      <c r="K24" s="54" t="n"/>
     </row>
     <row r="25" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A25" s="31" t="n">
@@ -2777,31 +2778,31 @@
       <c r="A26" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="60" t="n"/>
-      <c r="C26" s="60" t="n"/>
-      <c r="D26" s="60" t="n"/>
+      <c r="B26" s="54" t="n"/>
+      <c r="C26" s="54" t="n"/>
+      <c r="D26" s="54" t="n"/>
       <c r="E26" s="24" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="27" t="n"/>
       <c r="H26" s="28" t="n"/>
-      <c r="I26" s="60" t="n"/>
+      <c r="I26" s="54" t="n"/>
       <c r="J26" s="38" t="n"/>
-      <c r="K26" s="60" t="n"/>
+      <c r="K26" s="54" t="n"/>
     </row>
     <row r="27" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A27" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="49" t="n"/>
-      <c r="C27" s="49" t="n"/>
-      <c r="D27" s="49" t="n"/>
-      <c r="E27" s="52" t="n"/>
+      <c r="B27" s="50" t="n"/>
+      <c r="C27" s="50" t="n"/>
+      <c r="D27" s="50" t="n"/>
+      <c r="E27" s="64" t="n"/>
       <c r="F27" s="17" t="n"/>
-      <c r="G27" s="54" t="n"/>
+      <c r="G27" s="66" t="n"/>
       <c r="H27" s="20" t="n"/>
-      <c r="I27" s="49" t="n"/>
+      <c r="I27" s="50" t="n"/>
       <c r="J27" s="38" t="n"/>
-      <c r="K27" s="49" t="n"/>
+      <c r="K27" s="50" t="n"/>
     </row>
     <row r="28" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A28" s="11" t="n">
@@ -2916,7 +2917,7 @@
       <c r="C35" s="11" t="n"/>
       <c r="D35" s="11" t="n"/>
       <c r="E35" s="11" t="n"/>
-      <c r="F35" s="49" t="n"/>
+      <c r="F35" s="50" t="n"/>
       <c r="G35" s="11" t="n"/>
       <c r="H35" s="5" t="n"/>
       <c r="I35" s="11" t="n"/>
@@ -3008,12 +3009,12 @@
       <c r="G41" s="12" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="66" t="n"/>
-      <c r="C42" s="66" t="n"/>
-      <c r="D42" s="66" t="n"/>
-      <c r="E42" s="66" t="n"/>
-      <c r="F42" s="66" t="n"/>
-      <c r="G42" s="50" t="n"/>
+      <c r="A42" s="60" t="n"/>
+      <c r="C42" s="60" t="n"/>
+      <c r="D42" s="60" t="n"/>
+      <c r="E42" s="60" t="n"/>
+      <c r="F42" s="60" t="n"/>
+      <c r="G42" s="45" t="n"/>
       <c r="I42" s="46" t="n"/>
       <c r="J42" s="40" t="n"/>
       <c r="K42" s="9" t="n"/>
@@ -3037,12 +3038,12 @@
       <c r="I50" s="43" t="n"/>
     </row>
     <row r="51">
-      <c r="C51" s="62" t="inlineStr">
+      <c r="C51" s="56" t="inlineStr">
         <is>
           <t>Mtra. Lilibeth Hernández Alba</t>
         </is>
       </c>
-      <c r="D51" s="63" t="n"/>
+      <c r="D51" s="57" t="n"/>
       <c r="G51" s="47" t="inlineStr">
         <is>
           <t>Mtra. Dely Karolina Urbano Sanchez</t>
@@ -3050,12 +3051,12 @@
       </c>
     </row>
     <row r="52">
-      <c r="C52" s="50" t="inlineStr">
+      <c r="C52" s="45" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SEVICIOS ESCOLARES</t>
         </is>
       </c>
-      <c r="G52" s="50" t="inlineStr">
+      <c r="G52" s="45" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -3065,11 +3066,11 @@
   <mergeCells count="29">
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="J13:J14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C11:H11"/>
@@ -3107,7 +3108,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:D51"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -3121,19 +3122,19 @@
     <col width="20" customWidth="1" style="46" min="7" max="7"/>
     <col width="15.33203125" customWidth="1" style="47" min="8" max="8"/>
     <col width="19.1640625" customWidth="1" style="47" min="9" max="9"/>
-    <col width="16.5" customWidth="1" style="56" min="10" max="10"/>
+    <col width="16.5" customWidth="1" style="52" min="10" max="10"/>
     <col width="44.33203125" customWidth="1" style="47" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">
-      <c r="A1" s="55" t="inlineStr">
+      <c r="A1" s="61" t="inlineStr">
         <is>
           <t>UNIVERSIDAD ETAC ON ALIAT</t>
         </is>
       </c>
     </row>
     <row r="2" ht="26.25" customHeight="1">
-      <c r="A2" s="55" t="inlineStr">
+      <c r="A2" s="61" t="inlineStr">
         <is>
           <t>CAMPUS ÚNICO</t>
         </is>
@@ -3153,14 +3154,14 @@
       <c r="K3" s="1" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="57" t="inlineStr">
+      <c r="A4" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">SERVICIOS ESCOLARES </t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="57" t="inlineStr">
+      <c r="A6" s="51" t="inlineStr">
         <is>
           <t>LIBRO DE CONTROL DE FOLIOS DE TITULOS ELECTRONICOS</t>
         </is>
@@ -3173,8 +3174,8 @@
       <c r="K7" s="46" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="n"/>
-      <c r="C8" s="45" t="n"/>
+      <c r="A8" s="48" t="n"/>
+      <c r="C8" s="48" t="n"/>
       <c r="I8" s="4" t="inlineStr">
         <is>
           <t>FECHA</t>
@@ -3186,8 +3187,8 @@
       <c r="K8" s="6" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="45" t="n"/>
-      <c r="C9" s="45" t="n"/>
+      <c r="A9" s="48" t="n"/>
+      <c r="C9" s="48" t="n"/>
       <c r="I9" s="4" t="inlineStr">
         <is>
           <t>HOJA</t>
@@ -3201,18 +3202,18 @@
       <c r="K9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="45" t="n"/>
-      <c r="C10" s="45" t="n"/>
-      <c r="I10" s="45" t="n"/>
+      <c r="A10" s="48" t="n"/>
+      <c r="C10" s="48" t="n"/>
+      <c r="I10" s="48" t="n"/>
       <c r="J10" s="39" t="n"/>
-      <c r="K10" s="45" t="n"/>
+      <c r="K10" s="48" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="n"/>
-      <c r="C11" s="45" t="n"/>
-      <c r="I11" s="45" t="n"/>
+      <c r="A11" s="48" t="n"/>
+      <c r="C11" s="48" t="n"/>
+      <c r="I11" s="48" t="n"/>
       <c r="J11" s="39" t="n"/>
-      <c r="K11" s="45" t="n"/>
+      <c r="K11" s="48" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="n"/>
@@ -3228,74 +3229,74 @@
       <c r="K12" s="9" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="61" t="inlineStr">
+      <c r="A13" s="55" t="inlineStr">
         <is>
           <t>NUM. PROG.</t>
         </is>
       </c>
-      <c r="B13" s="58" t="inlineStr">
+      <c r="B13" s="49" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C13" s="58" t="inlineStr">
+      <c r="C13" s="49" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D13" s="58" t="inlineStr">
+      <c r="D13" s="49" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E13" s="51" t="inlineStr">
+      <c r="E13" s="63" t="inlineStr">
         <is>
           <t>CLAVE DE CARRERA</t>
         </is>
       </c>
-      <c r="F13" s="59" t="inlineStr">
+      <c r="F13" s="53" t="inlineStr">
         <is>
           <t>FOLIO DE CONTROL</t>
         </is>
       </c>
-      <c r="G13" s="53" t="inlineStr">
+      <c r="G13" s="65" t="inlineStr">
         <is>
           <t>LUGAR DE EXPEDICIÓN</t>
         </is>
       </c>
-      <c r="H13" s="61" t="inlineStr">
-        <is>
-          <t>FECHA DE EXPEDICIÓN</t>
-        </is>
-      </c>
-      <c r="I13" s="64" t="inlineStr">
+      <c r="H13" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I13" s="58" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J13" s="48" t="inlineStr">
+      <c r="J13" s="62" t="inlineStr">
         <is>
           <t>CLAVE DE INSTITUCIÓN</t>
         </is>
       </c>
-      <c r="K13" s="61" t="inlineStr">
+      <c r="K13" s="55" t="inlineStr">
         <is>
           <t>FOLIO DIGITAL</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="n"/>
-      <c r="B14" s="49" t="n"/>
-      <c r="C14" s="49" t="n"/>
-      <c r="D14" s="49" t="n"/>
-      <c r="E14" s="52" t="n"/>
-      <c r="F14" s="60" t="n"/>
-      <c r="G14" s="54" t="n"/>
-      <c r="H14" s="49" t="n"/>
-      <c r="I14" s="65" t="n"/>
-      <c r="J14" s="49" t="n"/>
-      <c r="K14" s="49" t="n"/>
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="50" t="n"/>
+      <c r="C14" s="50" t="n"/>
+      <c r="D14" s="50" t="n"/>
+      <c r="E14" s="64" t="n"/>
+      <c r="F14" s="54" t="n"/>
+      <c r="G14" s="66" t="n"/>
+      <c r="H14" s="50" t="n"/>
+      <c r="I14" s="59" t="n"/>
+      <c r="J14" s="50" t="n"/>
+      <c r="K14" s="50" t="n"/>
     </row>
     <row r="15" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A15" s="22" t="n">
@@ -3433,19 +3434,19 @@
       <c r="K23" s="15" t="n"/>
     </row>
     <row r="24" ht="20.25" customFormat="1" customHeight="1" s="47">
-      <c r="A24" s="52" t="n">
+      <c r="A24" s="64" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="60" t="n"/>
-      <c r="C24" s="60" t="n"/>
-      <c r="D24" s="60" t="n"/>
+      <c r="B24" s="54" t="n"/>
+      <c r="C24" s="54" t="n"/>
+      <c r="D24" s="54" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="17" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="28" t="n"/>
-      <c r="I24" s="60" t="n"/>
+      <c r="I24" s="54" t="n"/>
       <c r="J24" s="38" t="n"/>
-      <c r="K24" s="60" t="n"/>
+      <c r="K24" s="54" t="n"/>
     </row>
     <row r="25" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A25" s="31" t="n">
@@ -3466,31 +3467,31 @@
       <c r="A26" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="B26" s="60" t="n"/>
-      <c r="C26" s="60" t="n"/>
-      <c r="D26" s="60" t="n"/>
+      <c r="B26" s="54" t="n"/>
+      <c r="C26" s="54" t="n"/>
+      <c r="D26" s="54" t="n"/>
       <c r="E26" s="24" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="27" t="n"/>
       <c r="H26" s="28" t="n"/>
-      <c r="I26" s="60" t="n"/>
+      <c r="I26" s="54" t="n"/>
       <c r="J26" s="38" t="n"/>
-      <c r="K26" s="60" t="n"/>
+      <c r="K26" s="54" t="n"/>
     </row>
     <row r="27" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A27" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="49" t="n"/>
-      <c r="C27" s="49" t="n"/>
-      <c r="D27" s="49" t="n"/>
-      <c r="E27" s="52" t="n"/>
+      <c r="B27" s="50" t="n"/>
+      <c r="C27" s="50" t="n"/>
+      <c r="D27" s="50" t="n"/>
+      <c r="E27" s="64" t="n"/>
       <c r="F27" s="17" t="n"/>
-      <c r="G27" s="54" t="n"/>
+      <c r="G27" s="66" t="n"/>
       <c r="H27" s="20" t="n"/>
-      <c r="I27" s="49" t="n"/>
+      <c r="I27" s="50" t="n"/>
       <c r="J27" s="38" t="n"/>
-      <c r="K27" s="49" t="n"/>
+      <c r="K27" s="50" t="n"/>
     </row>
     <row r="28" ht="20.25" customFormat="1" customHeight="1" s="47">
       <c r="A28" s="11" t="n">
@@ -3605,7 +3606,7 @@
       <c r="C35" s="11" t="n"/>
       <c r="D35" s="11" t="n"/>
       <c r="E35" s="11" t="n"/>
-      <c r="F35" s="49" t="n"/>
+      <c r="F35" s="50" t="n"/>
       <c r="G35" s="11" t="n"/>
       <c r="H35" s="5" t="n"/>
       <c r="I35" s="11" t="n"/>
@@ -3697,12 +3698,12 @@
       <c r="G41" s="12" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="66" t="n"/>
-      <c r="C42" s="66" t="n"/>
-      <c r="D42" s="66" t="n"/>
-      <c r="E42" s="66" t="n"/>
-      <c r="F42" s="66" t="n"/>
-      <c r="G42" s="50" t="n"/>
+      <c r="A42" s="60" t="n"/>
+      <c r="C42" s="60" t="n"/>
+      <c r="D42" s="60" t="n"/>
+      <c r="E42" s="60" t="n"/>
+      <c r="F42" s="60" t="n"/>
+      <c r="G42" s="45" t="n"/>
       <c r="I42" s="46" t="n"/>
       <c r="J42" s="40" t="n"/>
       <c r="K42" s="9" t="n"/>
@@ -3726,12 +3727,12 @@
       <c r="I50" s="43" t="n"/>
     </row>
     <row r="51">
-      <c r="C51" s="62" t="inlineStr">
+      <c r="C51" s="56" t="inlineStr">
         <is>
           <t>F5</t>
         </is>
       </c>
-      <c r="D51" s="63" t="n"/>
+      <c r="D51" s="57" t="n"/>
       <c r="G51" s="47" t="inlineStr">
         <is>
           <t>Mtra. Dely Karolina Urbano Sanchez</t>
@@ -3739,12 +3740,12 @@
       </c>
     </row>
     <row r="52">
-      <c r="C52" s="50" t="inlineStr">
+      <c r="C52" s="45" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SEVICIOS ESCOLARES</t>
         </is>
       </c>
-      <c r="G52" s="50" t="inlineStr">
+      <c r="G52" s="45" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -3754,11 +3755,11 @@
   <mergeCells count="29">
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="J13:J14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C11:H11"/>
@@ -3793,7 +3794,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3828,174 +3829,150 @@
           <t>LIBRO DE CONTROL DE FOLIOS DE TÍTULOS ELECTRÓNICOS</t>
         </is>
       </c>
+      <c r="K6" s="69" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="L6" s="69" t="inlineStr">
+        <is>
+          <t>2025-01-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7" s="69" t="inlineStr">
+        <is>
+          <t>HOJA</t>
+        </is>
+      </c>
+      <c r="L7" s="69" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="69" t="inlineStr">
+      <c r="A14" s="70" t="inlineStr">
         <is>
           <t>NUM_PROG</t>
         </is>
       </c>
-      <c r="B14" s="69" t="inlineStr">
+      <c r="B14" s="70" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C14" s="69" t="inlineStr">
+      <c r="C14" s="70" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D14" s="69" t="inlineStr">
+      <c r="D14" s="70" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E14" s="69" t="inlineStr">
+      <c r="E14" s="70" t="inlineStr">
         <is>
           <t>CLAVE_DE_CARRERA</t>
         </is>
       </c>
-      <c r="F14" s="69" t="inlineStr">
+      <c r="F14" s="70" t="inlineStr">
         <is>
           <t>FOLIO_DE_CONTROL</t>
         </is>
       </c>
-      <c r="G14" s="69" t="inlineStr">
+      <c r="G14" s="70" t="inlineStr">
         <is>
           <t>LUGAR_DE_EXPEDICION</t>
         </is>
       </c>
-      <c r="H14" s="69" t="inlineStr">
+      <c r="H14" s="70" t="inlineStr">
         <is>
           <t>FECHA_DE_EXPEDICION</t>
         </is>
       </c>
-      <c r="I14" s="69" t="inlineStr">
+      <c r="I14" s="70" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J14" s="69" t="inlineStr">
+      <c r="J14" s="70" t="inlineStr">
         <is>
           <t>CLAVE_DE_INSTITUCION</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="69" t="n">
+      <c r="A15" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="69" t="inlineStr">
-        <is>
-          <t>AXEL DAMIAN HERNANDEZ LOZOYA</t>
-        </is>
-      </c>
-      <c r="C15" s="69" t="inlineStr">
-        <is>
-          <t>HELA000222HCHRZXA2</t>
-        </is>
-      </c>
-      <c r="D15" s="69" t="inlineStr">
-        <is>
-          <t>LICENCIATURA EN DERECHO</t>
-        </is>
-      </c>
-      <c r="E15" s="69" t="inlineStr">
-        <is>
-          <t>010157</t>
-        </is>
-      </c>
-      <c r="F15" s="69" t="inlineStr">
-        <is>
-          <t>ONALT_03_010157_00000310799_UGRV_0_01</t>
-        </is>
-      </c>
-      <c r="G15" s="69" t="inlineStr">
-        <is>
-          <t>AGUASCALIENTES</t>
-        </is>
-      </c>
-      <c r="H15" s="69" t="inlineStr">
-        <is>
-          <t>2025-02-13</t>
-        </is>
-      </c>
-      <c r="I15" s="69" t="inlineStr">
-        <is>
-          <t>20230244</t>
-        </is>
-      </c>
-      <c r="J15" s="69" t="inlineStr">
-        <is>
-          <t>010157</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="69" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" s="69" t="inlineStr">
-        <is>
-          <t>CARLOS ALEJANDRO HERNANDEZ ALVAREZ</t>
-        </is>
-      </c>
-      <c r="C16" s="69" t="inlineStr">
-        <is>
-          <t>HEAC010722HQTRLRA5</t>
-        </is>
-      </c>
-      <c r="D16" s="69" t="inlineStr">
-        <is>
-          <t>LICENCIATURA EN GASTRONOMÍA</t>
-        </is>
-      </c>
-      <c r="E16" s="69" t="inlineStr">
-        <is>
-          <t>010157</t>
-        </is>
-      </c>
-      <c r="F16" s="69" t="inlineStr">
-        <is>
-          <t>UNEAQ_01_010157_00000310262_UGRD_1_03</t>
-        </is>
-      </c>
-      <c r="G16" s="69" t="inlineStr">
-        <is>
-          <t>AGUASCALIENTES</t>
-        </is>
-      </c>
-      <c r="H16" s="69" t="inlineStr">
-        <is>
-          <t>2025-02-10</t>
-        </is>
-      </c>
-      <c r="I16" s="69" t="inlineStr">
-        <is>
-          <t>20230249</t>
-        </is>
-      </c>
-      <c r="J16" s="69" t="inlineStr">
-        <is>
-          <t>010157</t>
+      <c r="B15" s="70" t="inlineStr">
+        <is>
+          <t>NOEMI GUADALUPE FRAIRE PIZANO</t>
+        </is>
+      </c>
+      <c r="C15" s="70" t="inlineStr">
+        <is>
+          <t>FAPN850911MDFRZM07</t>
+        </is>
+      </c>
+      <c r="D15" s="70" t="inlineStr">
+        <is>
+          <t>MAESTRÍA EN GESTIÓN EDUCATIVA</t>
+        </is>
+      </c>
+      <c r="E15" s="70" t="inlineStr">
+        <is>
+          <t>150901</t>
+        </is>
+      </c>
+      <c r="F15" s="70" t="inlineStr">
+        <is>
+          <t>ETAV_05_150901_00000346333_MSTV_1_01</t>
+        </is>
+      </c>
+      <c r="G15" s="70" t="inlineStr">
+        <is>
+          <t>MÉXICO</t>
+        </is>
+      </c>
+      <c r="H15" s="70" t="inlineStr">
+        <is>
+          <t>2025-01-06</t>
+        </is>
+      </c>
+      <c r="I15" s="70" t="inlineStr">
+        <is>
+          <t>20192513</t>
+        </is>
+      </c>
+      <c r="J15" s="70" t="inlineStr">
+        <is>
+          <t>150901</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="69" t="inlineStr">
+        <is>
+          <t>Mtra. Beatriz Adriana Barron Linares</t>
+        </is>
+      </c>
+      <c r="I25" s="69" t="inlineStr">
+        <is>
+          <t>Mtra. Dely Karolina Urbano Sanchez</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="70" t="inlineStr"/>
-      <c r="I26" s="70" t="inlineStr">
-        <is>
-          <t>Mtra. Dely Karolina Urbano Sanchez</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="70" t="inlineStr">
+      <c r="B26" s="69" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SERVICIOS ESCOLARES</t>
         </is>
       </c>
-      <c r="I27" s="70" t="inlineStr">
+      <c r="I26" s="69" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -4003,12 +3980,12 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:L2"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="A6:J6"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="A4:L4"/>
   </mergeCells>
@@ -4057,174 +4034,200 @@
           <t>LIBRO DE CONTROL DE FOLIOS DE TÍTULOS ELECTRÓNICOS</t>
         </is>
       </c>
+      <c r="K6" s="69" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="L6" s="69" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7" s="69" t="inlineStr">
+        <is>
+          <t>HOJA</t>
+        </is>
+      </c>
+      <c r="L7" s="69" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="69" t="inlineStr">
+      <c r="A14" s="70" t="inlineStr">
         <is>
           <t>NUM_PROG</t>
         </is>
       </c>
-      <c r="B14" s="69" t="inlineStr">
+      <c r="B14" s="70" t="inlineStr">
         <is>
           <t>ALUMNO</t>
         </is>
       </c>
-      <c r="C14" s="69" t="inlineStr">
+      <c r="C14" s="70" t="inlineStr">
         <is>
           <t>CURP</t>
         </is>
       </c>
-      <c r="D14" s="69" t="inlineStr">
+      <c r="D14" s="70" t="inlineStr">
         <is>
           <t>PROGRAMA</t>
         </is>
       </c>
-      <c r="E14" s="69" t="inlineStr">
+      <c r="E14" s="70" t="inlineStr">
         <is>
           <t>CLAVE_DE_CARRERA</t>
         </is>
       </c>
-      <c r="F14" s="69" t="inlineStr">
+      <c r="F14" s="70" t="inlineStr">
         <is>
           <t>FOLIO_DE_CONTROL</t>
         </is>
       </c>
-      <c r="G14" s="69" t="inlineStr">
+      <c r="G14" s="70" t="inlineStr">
         <is>
           <t>LUGAR_DE_EXPEDICION</t>
         </is>
       </c>
-      <c r="H14" s="69" t="inlineStr">
+      <c r="H14" s="70" t="inlineStr">
         <is>
           <t>FECHA_DE_EXPEDICION</t>
         </is>
       </c>
-      <c r="I14" s="69" t="inlineStr">
+      <c r="I14" s="70" t="inlineStr">
         <is>
           <t>RVOE</t>
         </is>
       </c>
-      <c r="J14" s="69" t="inlineStr">
+      <c r="J14" s="70" t="inlineStr">
         <is>
           <t>CLAVE_DE_INSTITUCION</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="69" t="n">
+      <c r="A15" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="69" t="inlineStr">
-        <is>
-          <t>MARIA DEL ROSARIO DE LA CRUZ MUÑOZ</t>
-        </is>
-      </c>
-      <c r="C15" s="69" t="inlineStr">
-        <is>
-          <t>CUMR741224MDFRXS05</t>
-        </is>
-      </c>
-      <c r="D15" s="69" t="inlineStr">
-        <is>
-          <t>MAESTRÍA EN DOCENCIA</t>
-        </is>
-      </c>
-      <c r="E15" s="69" t="inlineStr">
+      <c r="B15" s="70" t="inlineStr">
+        <is>
+          <t>MARISOL SOTO GONZALEZ</t>
+        </is>
+      </c>
+      <c r="C15" s="70" t="inlineStr">
+        <is>
+          <t>SOGM860716MMCTNR08</t>
+        </is>
+      </c>
+      <c r="D15" s="70" t="inlineStr">
+        <is>
+          <t>LICENCIATURA EN ADMINISTRACIÓN DE EMPRESAS</t>
+        </is>
+      </c>
+      <c r="E15" s="70" t="inlineStr">
         <is>
           <t>150901</t>
         </is>
       </c>
-      <c r="F15" s="69" t="inlineStr">
-        <is>
-          <t>B2B_06_150901_00000004983_MSTV_1_01</t>
-        </is>
-      </c>
-      <c r="G15" s="69" t="inlineStr">
+      <c r="F15" s="70" t="inlineStr">
+        <is>
+          <t>B2B_06_150901_00000313668_UGRV_0_01</t>
+        </is>
+      </c>
+      <c r="G15" s="70" t="inlineStr">
         <is>
           <t>MÉXICO</t>
         </is>
       </c>
-      <c r="H15" s="69" t="inlineStr">
-        <is>
-          <t>2025-04-30</t>
-        </is>
-      </c>
-      <c r="I15" s="69" t="inlineStr">
-        <is>
-          <t>20192511</t>
-        </is>
-      </c>
-      <c r="J15" s="69" t="inlineStr">
+      <c r="H15" s="70" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
+      <c r="I15" s="70" t="inlineStr">
+        <is>
+          <t>20170654</t>
+        </is>
+      </c>
+      <c r="J15" s="70" t="inlineStr">
         <is>
           <t>150901</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="69" t="n">
+      <c r="A16" s="70" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="69" t="inlineStr">
-        <is>
-          <t>ERICK BERNARDO CORDOVA</t>
-        </is>
-      </c>
-      <c r="C16" s="69" t="inlineStr">
-        <is>
-          <t>BECE910302HTCRRR08</t>
-        </is>
-      </c>
-      <c r="D16" s="69" t="inlineStr">
+      <c r="B16" s="70" t="inlineStr">
+        <is>
+          <t>ADAN MARTINEZ GONZALEZ</t>
+        </is>
+      </c>
+      <c r="C16" s="70" t="inlineStr">
+        <is>
+          <t>MAGA771017HMCRND01</t>
+        </is>
+      </c>
+      <c r="D16" s="70" t="inlineStr">
         <is>
           <t>LICENCIATURA EN INGENIERÍA INDUSTRIAL</t>
         </is>
       </c>
-      <c r="E16" s="69" t="inlineStr">
-        <is>
-          <t>010162</t>
-        </is>
-      </c>
-      <c r="F16" s="69" t="inlineStr">
-        <is>
-          <t>ONALT_02_010162_00000297211_UGRV_0_02</t>
-        </is>
-      </c>
-      <c r="G16" s="69" t="inlineStr">
-        <is>
-          <t>AGUASCALIENTES</t>
-        </is>
-      </c>
-      <c r="H16" s="69" t="inlineStr">
-        <is>
-          <t>2025-04-30</t>
-        </is>
-      </c>
-      <c r="I16" s="69" t="inlineStr">
-        <is>
-          <t>20230287</t>
-        </is>
-      </c>
-      <c r="J16" s="69" t="inlineStr">
-        <is>
-          <t>010162</t>
+      <c r="E16" s="70" t="inlineStr">
+        <is>
+          <t>150901</t>
+        </is>
+      </c>
+      <c r="F16" s="70" t="inlineStr">
+        <is>
+          <t>B2B_06_150901_00000321660_UGRV_0_01</t>
+        </is>
+      </c>
+      <c r="G16" s="70" t="inlineStr">
+        <is>
+          <t>MÉXICO</t>
+        </is>
+      </c>
+      <c r="H16" s="70" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
+      <c r="I16" s="70" t="inlineStr">
+        <is>
+          <t>20170434</t>
+        </is>
+      </c>
+      <c r="J16" s="70" t="inlineStr">
+        <is>
+          <t>150901</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="70" t="inlineStr"/>
-      <c r="I26" s="70" t="inlineStr">
+      <c r="B26" s="69" t="inlineStr">
+        <is>
+          <t>Mtra. Beatriz Adriana Barron Linares</t>
+        </is>
+      </c>
+      <c r="I26" s="69" t="inlineStr">
         <is>
           <t>Mtra. Dely Karolina Urbano Sanchez</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="70" t="inlineStr">
+      <c r="B27" s="69" t="inlineStr">
         <is>
           <t>RESPONSABLE DE SERVICIOS ESCOLARES</t>
         </is>
       </c>
-      <c r="I27" s="70" t="inlineStr">
+      <c r="I27" s="69" t="inlineStr">
         <is>
           <t>RECTOR</t>
         </is>
@@ -4233,11 +4236,266 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A2:L2"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A6:J6"/>
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="A4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="67" t="inlineStr">
+        <is>
+          <t>UNIVERSIDAD ETAC ON ALIAT</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="68" t="inlineStr">
+        <is>
+          <t>CAMPUS ÚNICO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="68" t="inlineStr">
+        <is>
+          <t>SERVICIOS ESCOLARES</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="68" t="inlineStr">
+        <is>
+          <t>LIBRO DE CONTROL DE FOLIOS DE TÍTULOS ELECTRÓNICOS</t>
+        </is>
+      </c>
+      <c r="K6" s="69" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="L6" s="69" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7" s="69" t="inlineStr">
+        <is>
+          <t>HOJA</t>
+        </is>
+      </c>
+      <c r="L7" s="69" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="70" t="inlineStr">
+        <is>
+          <t>NUM_PROG</t>
+        </is>
+      </c>
+      <c r="B14" s="70" t="inlineStr">
+        <is>
+          <t>ALUMNO</t>
+        </is>
+      </c>
+      <c r="C14" s="70" t="inlineStr">
+        <is>
+          <t>CURP</t>
+        </is>
+      </c>
+      <c r="D14" s="70" t="inlineStr">
+        <is>
+          <t>PROGRAMA</t>
+        </is>
+      </c>
+      <c r="E14" s="70" t="inlineStr">
+        <is>
+          <t>CLAVE_DE_CARRERA</t>
+        </is>
+      </c>
+      <c r="F14" s="70" t="inlineStr">
+        <is>
+          <t>FOLIO_DE_CONTROL</t>
+        </is>
+      </c>
+      <c r="G14" s="70" t="inlineStr">
+        <is>
+          <t>LUGAR_DE_EXPEDICION</t>
+        </is>
+      </c>
+      <c r="H14" s="70" t="inlineStr">
+        <is>
+          <t>FECHA_DE_EXPEDICION</t>
+        </is>
+      </c>
+      <c r="I14" s="70" t="inlineStr">
+        <is>
+          <t>RVOE</t>
+        </is>
+      </c>
+      <c r="J14" s="70" t="inlineStr">
+        <is>
+          <t>CLAVE_DE_INSTITUCION</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="70" t="inlineStr">
+        <is>
+          <t>KARLA GUADALUPE CASTRO FLORES</t>
+        </is>
+      </c>
+      <c r="C15" s="70" t="inlineStr">
+        <is>
+          <t>CAFK980830MSLSLR08</t>
+        </is>
+      </c>
+      <c r="D15" s="70" t="inlineStr">
+        <is>
+          <t>LICENCIATURA EN CRIMINALÍSTICA</t>
+        </is>
+      </c>
+      <c r="E15" s="70" t="inlineStr">
+        <is>
+          <t>010157</t>
+        </is>
+      </c>
+      <c r="F15" s="70" t="inlineStr">
+        <is>
+          <t>ONALT_03_010157_00000304009_UGRV_0_02</t>
+        </is>
+      </c>
+      <c r="G15" s="70" t="inlineStr">
+        <is>
+          <t>AGUASCALIENTES</t>
+        </is>
+      </c>
+      <c r="H15" s="70" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+      <c r="I15" s="70" t="inlineStr">
+        <is>
+          <t>20230243</t>
+        </is>
+      </c>
+      <c r="J15" s="70" t="inlineStr">
+        <is>
+          <t>010157</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="70" t="inlineStr">
+        <is>
+          <t>GABRIELA VALENZUELA CASTAÑEDA</t>
+        </is>
+      </c>
+      <c r="C16" s="70" t="inlineStr">
+        <is>
+          <t>VACG840411MBCLSB06</t>
+        </is>
+      </c>
+      <c r="D16" s="70" t="inlineStr">
+        <is>
+          <t>LICENCIATURA EN DERECHO</t>
+        </is>
+      </c>
+      <c r="E16" s="70" t="inlineStr">
+        <is>
+          <t>010157</t>
+        </is>
+      </c>
+      <c r="F16" s="70" t="inlineStr">
+        <is>
+          <t>ONALT_03_010157_00000321708_UGRV_0_02</t>
+        </is>
+      </c>
+      <c r="G16" s="70" t="inlineStr">
+        <is>
+          <t>AGUASCALIENTES</t>
+        </is>
+      </c>
+      <c r="H16" s="70" t="inlineStr">
+        <is>
+          <t>2024-12-01</t>
+        </is>
+      </c>
+      <c r="I16" s="70" t="inlineStr">
+        <is>
+          <t>20230244</t>
+        </is>
+      </c>
+      <c r="J16" s="70" t="inlineStr">
+        <is>
+          <t>010157</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="69" t="inlineStr">
+        <is>
+          <t>Mtra. Lilibeth Hernandez Alva</t>
+        </is>
+      </c>
+      <c r="I26" s="69" t="inlineStr">
+        <is>
+          <t>Mtra. Dely Karolina Urbano Sanchez</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="69" t="inlineStr">
+        <is>
+          <t>RESPONSABLE DE SERVICIOS ESCOLARES</t>
+        </is>
+      </c>
+      <c r="I27" s="69" t="inlineStr">
+        <is>
+          <t>RECTOR</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="A4:L4"/>
   </mergeCells>

</xml_diff>